<commit_message>
Remove binary file for xlsx
</commit_message>
<xml_diff>
--- a/Syllabus/schedule.xlsx
+++ b/Syllabus/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avahoffman/Dropbox/JHSPH/intro_to_r/Syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D72B30C-78CA-E845-99CD-652260B5E38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACD2BBC-DA63-0346-AA59-3CD78EACD89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-15100" windowWidth="37540" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1097,7 +1097,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>